<commit_message>
Initial commit in correct project folder
</commit_message>
<xml_diff>
--- a/test-data/TestData.xlsx
+++ b/test-data/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7980" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7980"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Phone</t>
   </si>
@@ -36,10 +36,46 @@
     <t>OTP</t>
   </si>
   <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>01510000239</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>test@me.com</t>
+  </si>
+  <si>
+    <t>Test Company Ltd</t>
+  </si>
+  <si>
     <t>01400000001</t>
   </si>
   <si>
-    <t>1234</t>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>john.doe@example.com</t>
   </si>
   <si>
     <t>Product Name</t>
@@ -79,7 +115,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +136,13 @@
       <color rgb="FF253D4E"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF212529"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -572,137 +615,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -718,11 +761,26 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="6" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" quotePrefix="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1257,35 +1315,88 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.02654867256637" defaultRowHeight="14.25" outlineLevelRow="2" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.6637168141593" style="5"/>
-    <col min="2" max="16384" width="9.02654867256637" style="5"/>
+    <col min="1" max="1" width="13.6106194690265" style="6" customWidth="1"/>
+    <col min="2" max="2" width="5.53097345132743" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.2477876106195" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.97345132743363" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21.8318584070796" style="6" customWidth="1"/>
+    <col min="6" max="6" width="16.1769911504425" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="9.02654867256637" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="1" spans="1:2">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="4" customFormat="1" spans="1:6">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
+    <row r="2" ht="15.75" spans="1:6">
+      <c r="A2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" s="5" customFormat="1" spans="1:6">
+      <c r="A3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="test@me.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="john.doe@example.com"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -1296,7 +1407,7 @@
   <sheetPr/>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
+    <sheetView zoomScaleSheetLayoutView="60" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1310,21 +1421,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>185</v>
@@ -1339,7 +1450,7 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1">
         <v>21</v>
@@ -1354,16 +1465,16 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>